<commit_message>
přidán zdroj Falešný Autostop
</commit_message>
<xml_diff>
--- a/cjl-knihy.xlsx
+++ b/cjl-knihy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Maturitka\CJL\excelTable\excelTabulkaLiteraturyNaMaturitu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F32F7D1-A2A5-4C51-BC84-91564DB87E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FB52E2-7C40-493B-9AA5-78A17BF8081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94871187-8663-4E32-9055-774820EF964F}"/>
   </bookViews>
@@ -542,7 +542,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -590,236 +590,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1155,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08A221A-4539-429B-94E8-A725B3A71C58}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,7 +1915,7 @@
       <c r="C55" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="4" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2495,7 +2265,7 @@
     <mergeCell ref="A31:D31"/>
     <mergeCell ref="A48:D48"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:H48 H2">
+  <conditionalFormatting sqref="H2 H4:H48">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Splněn počet"</formula>
     </cfRule>
@@ -2581,8 +2351,9 @@
     <hyperlink ref="E12" r:id="rId64" xr:uid="{71F7DE5C-CF1E-4A37-B309-71A788F5B48E}"/>
     <hyperlink ref="E14" r:id="rId65" xr:uid="{A7727268-7A75-48B2-B8B3-4B2DDECD0DF5}"/>
     <hyperlink ref="E15" r:id="rId66" xr:uid="{F3BB44FD-00D2-492E-B4BC-17F4122E60D4}"/>
+    <hyperlink ref="E55" r:id="rId67" xr:uid="{A3F80129-AC15-49BA-866C-0B9DDC8A456C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId67"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId68"/>
 </worksheet>
 </file>
</xml_diff>